<commit_message>
Added start process function
</commit_message>
<xml_diff>
--- a/main/new.xlsx
+++ b/main/new.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:BH1"/>
+  <dimension ref="B1:BN1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,295 +436,325 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.5</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.4</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Company_Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Updating_Date</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Logo in Visualization folder?</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Operation Status (Active=True, False = False)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>INCLUSION</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Operation/relevant Notes</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>https://www.ibcheckpoint.com/</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Startup Nation Page</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Neurotech_Category</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Market_Category</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Target_Market</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>TechTools_1</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>TechTools_2</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>TechTools_3</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 14</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Full Description</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>CB (Crunchbase) Link</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Company CB Categories</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Company_Location</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Company_Founded_Year</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Company_Number_of_Employees</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Company_CB_Rank</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Funding_Status</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Last_Funding_Type</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Last_Funding_Date</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Last_Funding_Amount</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Total_Funding_Amount</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Total_Funding_Amount_M_dollars</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Number_of_Funding_Rounds</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Estimated_Revenue_Range</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Company_Number_of_Investors</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Company_Number_of_Investments</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Company LinkedIn Link</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Company_LinkedIn_Followers_Number</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Company Contact Email</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Company phone number</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Founders</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">CSO </t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>CTO</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>CEO</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>COO</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>CFO</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Co-Founder</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>President</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>Team Members</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>former company names</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>acquired</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>product_stage</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Number of Patents </t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Comments</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 52</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>Contact Name</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BJ1" s="1" t="inlineStr">
         <is>
           <t>Contact Phone Number / Email</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>האם יצרנו איתם כבר קשר? (כדי לא להתיש)</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>BrainstormIL contact</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 57</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 58</t>
         </is>

</xml_diff>